<commit_message>
Update homepage to reflect current HKUST position and add navigation bar
- Update intro section to show current Assistant Professor position at HKUST
- Simplify hiring announcement to reflect already started position
- Add fixed navigation bar with links to all major sections
- Add smooth scrolling and proper scroll offset for navigation
- Include Chinese name in navigation bar and page title
- Update local server port to 8001

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mingxunz/Documents/wuwuz.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F73EDA5-014A-AB4C-A469-F725BE6E578C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDDF0F8-2307-A540-B124-39A981CA69C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Publications" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="102">
   <si>
     <t>Year</t>
   </si>
@@ -322,6 +322,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ashrujit Ghoshal, Mingxun Zhou, Bo Peng, Elaine Shi </t>
+  </si>
+  <si>
+    <t>Bifrost: A Much Simpler Secure Two-Party Data Join Protocol for Secure Data Analytics</t>
+  </si>
+  <si>
+    <t>Shuyu Chen, Mingxun Zhou, Haoyu Niu, Guopeng Lin, Weili Han</t>
   </si>
 </sst>
 </file>
@@ -682,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -723,43 +729,37 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
+      <c r="A2">
+        <v>2026</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>97</v>
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
+      <c r="A3">
+        <v>2026</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -767,53 +767,56 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>99</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -821,19 +824,16 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -841,33 +841,36 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -875,22 +878,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -898,81 +898,121 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
         <v>43</v>
       </c>
-      <c r="G13" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>54</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
         <v>57</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E16" t="s">
         <v>58</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F16" t="s">
         <v>43</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -983,9 +1023,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1018,54 +1060,40 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" t="s">
         <v>48</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E4" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>